<commit_message>
Tons of weapon, melee kicks,
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -47,13 +47,40 @@
   </si>
   <si>
     <t>Готовность</t>
+  </si>
+  <si>
+    <t>Маски ударов</t>
+  </si>
+  <si>
+    <t>Двойной удар афины</t>
+  </si>
+  <si>
+    <t>3 удар крит у топора</t>
+  </si>
+  <si>
+    <t>Больше оружия</t>
+  </si>
+  <si>
+    <t>ИИ</t>
+  </si>
+  <si>
+    <t>Генерация уровней</t>
+  </si>
+  <si>
+    <t>Сундуки</t>
+  </si>
+  <si>
+    <t>Покупки</t>
+  </si>
+  <si>
+    <t>Хитбоксы и кикбоксы</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +104,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -145,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -153,6 +193,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Заголовок 2" xfId="1" builtinId="17"/>
@@ -643,16 +688,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -696,7 +741,66 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New weapon, ranged angle WIP
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -195,7 +195,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -691,7 +691,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Melee weapons animations wip
Middle commit
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -185,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -198,6 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Заголовок 2" xfId="1" builtinId="17"/>
@@ -691,7 +692,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -799,7 +800,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="7"/>
+      <c r="C14" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bitmask collision, wall shoot limit
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -399,6 +399,128 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5400675" y="2324100"/>
+          <a:ext cx="3676650" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>В сетке</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t> используется побитовое задание свойств клетки — каждая имеет несколько свойств -  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>SOLID, FLOOR, WALL, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>и т.д.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>Поэтому задание необходимо делать в форме</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>X | Y |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> .. | Z</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>В функцию </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>colPlaceFree </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>передавать точно так же</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>Игрок не ходит</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t> через </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>SOLID</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -691,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,14 +876,14 @@
         <v>12</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -782,12 +904,14 @@
         <v>16</v>
       </c>
       <c r="B11" s="5"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Rooms, random weapons, bues on floor
Random weapon generations still in progress, default rooms done
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Хитбоксы и кикбоксы</t>
+  </si>
+  <si>
+    <t>Мультиплеер</t>
+  </si>
+  <si>
+    <t>Кооператив</t>
+  </si>
+  <si>
+    <t>УДАЛЕНИП КАСТОМНЫХ СПРАЙТОВ</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,24 @@
     <cellStyle name="Заголовок 2" xfId="1" builtinId="17"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -811,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,24 +892,24 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -894,39 +920,61 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A6:C16">
+    <sortCondition sortBy="cellColor" ref="B6:B16" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="C6:C16" dxfId="0"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Shadows, fox, lasers on center
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>УДАЛЕНИП КАСТОМНЫХ СПРАЙТОВ</t>
+  </si>
+  <si>
+    <t>Оптимизация ИИ</t>
   </si>
 </sst>
 </file>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,10 +968,17 @@
       <c r="B16" s="5"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A6:C16">

</xml_diff>

<commit_message>
Bugs, weapons and CactusMan
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Оптимизация ИИ</t>
+  </si>
+  <si>
+    <t>Застревание пил в врагах</t>
+  </si>
+  <si>
+    <t>Отталкивания (игрок, враг, сущность)</t>
   </si>
 </sst>
 </file>
@@ -421,6 +427,32 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            * </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>gameGetWeaponInformation()</a:t>
           </a:r>
           <a:endParaRPr lang="ru-RU" sz="1100"/>
         </a:p>
@@ -840,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,17 +1000,30 @@
       <c r="B16" s="5"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A6:C16">

</xml_diff>

<commit_message>
AI, Boss sprites, octopus
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -92,13 +92,16 @@
   </si>
   <si>
     <t>Отталкивания (игрок, враг, сущность)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЕРЕЗАРЯДКА </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +136,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -217,12 +227,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Заголовок 2" xfId="1" builtinId="17"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -872,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,87 +991,93 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B21" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A6:C16">
-    <sortCondition sortBy="cellColor" ref="B6:B16" dxfId="1"/>
-    <sortCondition sortBy="cellColor" ref="C6:C16" dxfId="0"/>
+  <sortState ref="A6:C21">
+    <sortCondition sortBy="cellColor" ref="B6" dxfId="1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Octo club, octo healer
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,6 +1074,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A6:C21">

</xml_diff>

<commit_message>
Boss Molotov, new Minigun pattern
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Задачи по приоритетам:</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">ПЕРЕЗАРЯДКА </t>
+  </si>
+  <si>
+    <t>ОТКРЫВАТЬ ВСЕ ДВЕРИ В КОМНАТЕ 2 на 2</t>
   </si>
 </sst>
 </file>
@@ -233,47 +236,7 @@
     <cellStyle name="Заголовок 2" xfId="1" builtinId="17"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -915,15 +878,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D15:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -1076,9 +1039,16 @@
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+    </row>
   </sheetData>
   <sortState ref="A6:C21">
-    <sortCondition sortBy="cellColor" ref="B6" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="B6" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>